<commit_message>
Nueva pestaña para Auditar rechazos
</commit_message>
<xml_diff>
--- a/rechazos.xlsx
+++ b/rechazos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imail\OneDrive\Desktop\CODIGO ESTADIAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/904702f6d0479124/Desktop/CODIGO ESTADIAS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558E940E-CF3D-4777-BE19-43B9CE9AEEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{558E940E-CF3D-4777-BE19-43B9CE9AEEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D62320C-2E61-4226-8C64-479FF71F02F6}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{7748B0ED-53CC-47E5-8021-E1DAD9CF09DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7748B0ED-53CC-47E5-8021-E1DAD9CF09DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Rechazos" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>Fecha Rechazo</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>JESUS ALFREDO LIMAS ENCINAS</t>
+  </si>
+  <si>
+    <t>Comentarios</t>
   </si>
 </sst>
 </file>
@@ -162,7 +165,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -185,18 +188,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -207,6 +235,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{419A3D10-902A-4460-A51F-4E7953AAB501}" name="Tabla1" displayName="Tabla1" ref="A1:G18" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:G18" xr:uid="{419A3D10-902A-4460-A51F-4E7953AAB501}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{4A0E37DB-7769-4B46-94E3-C3829C5E9EA1}" name="Fecha Rechazo"/>
+    <tableColumn id="2" xr3:uid="{2BE93FB5-5325-49F2-B55E-C44D6380178E}" name="Sección"/>
+    <tableColumn id="3" xr3:uid="{817B8F88-5081-4EB0-B21F-888E0EFA2190}" name="Remisión"/>
+    <tableColumn id="4" xr3:uid="{7BD5A749-81D7-4C7C-86C1-C53FF792733F}" name="Sku"/>
+    <tableColumn id="5" xr3:uid="{2A270300-88B2-4422-8BF5-E835B01291FB}" name="Usuario"/>
+    <tableColumn id="6" xr3:uid="{C8ED93AB-0401-4C01-A6C8-2A8B4718A533}" name="Jefe"/>
+    <tableColumn id="7" xr3:uid="{32651D51-379E-4ABB-8082-389236BEAA81}" name="Comentarios"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -506,21 +550,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D533E90E-54A9-4879-9E12-9E0FD680E6E0}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:F19"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,8 +584,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -560,7 +608,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -580,7 +628,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -600,7 +648,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -620,58 +668,58 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B6">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="C6">
-        <v>7720058585</v>
+        <v>800057928</v>
       </c>
       <c r="D6">
-        <v>1113670084</v>
+        <v>1156914416</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>237</v>
       </c>
       <c r="C7">
-        <v>800057928</v>
+        <v>4500058427</v>
       </c>
       <c r="D7">
-        <v>1156914416</v>
+        <v>1103939166</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>237</v>
       </c>
       <c r="C8">
-        <v>4500058427</v>
+        <v>5530058565</v>
       </c>
       <c r="D8">
-        <v>1103939166</v>
+        <v>1153214715</v>
       </c>
       <c r="E8" t="s">
         <v>28</v>
@@ -680,78 +728,78 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="C9">
-        <v>5530058565</v>
+        <v>190058306</v>
       </c>
       <c r="D9">
-        <v>1153214715</v>
+        <v>1148925182</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10">
         <v>261</v>
       </c>
       <c r="C10">
-        <v>190058306</v>
+        <v>5530058638</v>
       </c>
       <c r="D10">
-        <v>1148925182</v>
+        <v>1158415816</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>261</v>
       </c>
       <c r="C11">
-        <v>5530058638</v>
+        <v>8590058677</v>
       </c>
       <c r="D11">
-        <v>1158415816</v>
+        <v>1148932952</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>261</v>
       </c>
       <c r="C12">
-        <v>8590058677</v>
+        <v>5270058194</v>
       </c>
       <c r="D12">
-        <v>1148932952</v>
+        <v>1141883158</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
@@ -760,38 +808,38 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>261</v>
       </c>
       <c r="C13">
-        <v>5270058194</v>
+        <v>3690058337</v>
       </c>
       <c r="D13">
-        <v>1141883158</v>
+        <v>1158420046</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>261</v>
       </c>
       <c r="C14">
-        <v>3690058337</v>
+        <v>4340058270</v>
       </c>
       <c r="D14">
-        <v>1158420046</v>
+        <v>1158412027</v>
       </c>
       <c r="E14" t="s">
         <v>30</v>
@@ -800,18 +848,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <v>261</v>
       </c>
       <c r="C15">
-        <v>4340058270</v>
+        <v>7900058413</v>
       </c>
       <c r="D15">
-        <v>1158412027</v>
+        <v>1163310909</v>
       </c>
       <c r="E15" t="s">
         <v>30</v>
@@ -820,88 +868,71 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16">
-        <v>261</v>
+        <v>550</v>
       </c>
       <c r="C16">
-        <v>7900058413</v>
+        <v>4850058246</v>
       </c>
       <c r="D16">
-        <v>1163310909</v>
+        <v>1081012411</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17">
-        <v>550</v>
+        <v>705</v>
       </c>
       <c r="C17">
-        <v>4850058246</v>
+        <v>7070058624</v>
       </c>
       <c r="D17">
-        <v>1081012411</v>
+        <v>1158955187</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="F17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B18">
-        <v>705</v>
+        <v>223</v>
       </c>
       <c r="C18">
-        <v>7070058624</v>
+        <v>7150058481</v>
       </c>
       <c r="D18">
-        <v>1158955187</v>
+        <v>1158950169</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="F18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19">
-        <v>223</v>
-      </c>
-      <c r="C19">
-        <v>7150058481</v>
-      </c>
-      <c r="D19">
-        <v>1158950169</v>
-      </c>
-      <c r="E19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>